<commit_message>
Updated PCB to use 5v power for the relay instead of 9v
</commit_message>
<xml_diff>
--- a/GuitarPedal125b/pcb/BOM_JLCSMT_DaisySeedGuitarPedal125b.xlsx
+++ b/GuitarPedal125b/pcb/BOM_JLCSMT_DaisySeedGuitarPedal125b.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshep/Dev/DaisySeedProjects/GuitarPedal125b/pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3F9187-FF10-6B49-83A2-CC2159F4B163}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CB98ED-046E-5348-B8D9-6591DFB4635D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37760" yWindow="4480" windowWidth="28800" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50940" yWindow="3120" windowWidth="28800" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>Comment</t>
   </si>
@@ -274,6 +274,57 @@
   </si>
   <si>
     <t>10K</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>G6K-2G-Y DC5</t>
+  </si>
+  <si>
+    <t>K1, K2</t>
+  </si>
+  <si>
+    <t>C397140</t>
+  </si>
+  <si>
+    <t>SMD,6.5x10mm</t>
+  </si>
+  <si>
+    <t>C78588</t>
+  </si>
+  <si>
+    <t>DIP-6</t>
+  </si>
+  <si>
+    <t>H11L1</t>
+  </si>
+  <si>
+    <t>PJ-320A</t>
+  </si>
+  <si>
+    <t>J4, J5</t>
+  </si>
+  <si>
+    <t>C2884926</t>
+  </si>
+  <si>
+    <t>J2, J3</t>
+  </si>
+  <si>
+    <t>C368502 or C309277</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2 or PJ-609BA</t>
+  </si>
+  <si>
+    <t>DC-005-2.5A-2.0</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>C319099</t>
   </si>
 </sst>
 </file>
@@ -379,7 +430,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -418,6 +469,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -762,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>
@@ -888,207 +942,265 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20" customHeight="1">
+      <c r="A13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5">
-        <v>805</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="C13" s="5">
+        <v>805</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20" customHeight="1">
-      <c r="A10" s="12" t="s">
+    <row r="14" spans="1:4" ht="20" customHeight="1">
+      <c r="A14" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="20" customHeight="1">
-      <c r="A11" s="11" t="s">
+    <row r="15" spans="1:4" ht="20" customHeight="1">
+      <c r="A15" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="5">
-        <v>805</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="C15" s="5">
+        <v>805</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="20" customHeight="1">
-      <c r="A12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="5">
-        <v>805</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="20" customHeight="1">
-      <c r="A13" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="5">
-        <v>805</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="20" customHeight="1">
-      <c r="A14" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="5">
-        <v>805</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="20" customHeight="1">
-      <c r="A15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="5">
-        <v>805</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="20" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5">
         <v>805</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C17" s="5">
         <v>805</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="20" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C18" s="5">
         <v>805</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="20" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="C19" s="5">
         <v>805</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="C20" s="5">
+        <v>805</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>49</v>
+        <v>40</v>
+      </c>
+      <c r="C21" s="5">
+        <v>805</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20" customHeight="1">
       <c r="A22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="5">
+        <v>805</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="20" customHeight="1">
+      <c r="A23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="5">
+        <v>805</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="20" customHeight="1">
+      <c r="A24" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="20" customHeight="1">
+      <c r="A25" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="20" customHeight="1">
+      <c r="A26" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="20" customHeight="1">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
+    <row r="27" spans="1:4" ht="20" customHeight="1">
+      <c r="A27" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
125B Guitar Pedal Rev 2
Updated the 125B Guitar Pedal to fix some issues, upgrade from 3 to 6 knobs and reposition the screen, and make it easier to manufacture with JLCPCB.
</commit_message>
<xml_diff>
--- a/GuitarPedal125b/pcb/BOM_JLCSMT_DaisySeedGuitarPedal125b.xlsx
+++ b/GuitarPedal125b/pcb/BOM_JLCSMT_DaisySeedGuitarPedal125b.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshep/Dev/DaisySeedProjects/GuitarPedal125b/pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CB98ED-046E-5348-B8D9-6591DFB4635D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAE0C70-2DCE-CB4F-BBD6-56C1240D3B6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50940" yWindow="3120" windowWidth="28800" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68540" yWindow="3140" windowWidth="28800" windowHeight="21660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
   <si>
     <t>Comment</t>
   </si>
@@ -156,9 +156,6 @@
     <t>C17408</t>
   </si>
   <si>
-    <t>R15, R19, R20</t>
-  </si>
-  <si>
     <t>C17557</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
     <t>C17513</t>
   </si>
   <si>
-    <t>R21</t>
-  </si>
-  <si>
     <t>C17414</t>
   </si>
   <si>
@@ -291,12 +285,6 @@
     <t>SMD,6.5x10mm</t>
   </si>
   <si>
-    <t>C78588</t>
-  </si>
-  <si>
-    <t>DIP-6</t>
-  </si>
-  <si>
     <t>H11L1</t>
   </si>
   <si>
@@ -312,26 +300,47 @@
     <t>J2, J3</t>
   </si>
   <si>
-    <t>C368502 or C309277</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2 or PJ-609BA</t>
-  </si>
-  <si>
     <t>DC-005-2.5A-2.0</t>
   </si>
   <si>
     <t>J1</t>
   </si>
   <si>
-    <t>C319099</t>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R19, R20, R21</t>
+  </si>
+  <si>
+    <t>C78589</t>
+  </si>
+  <si>
+    <t>SOP-6-2.54mm</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>C368502</t>
+  </si>
+  <si>
+    <t>C136744</t>
+  </si>
+  <si>
+    <t>PDS1-S5-S5-M</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>C5377809</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -381,6 +390,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -430,7 +458,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -471,6 +499,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -816,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>
@@ -908,46 +945,46 @@
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
@@ -956,40 +993,40 @@
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -1008,7 +1045,7 @@
     </row>
     <row r="14" spans="1:4" ht="20" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>25</v>
@@ -1022,7 +1059,7 @@
     </row>
     <row r="15" spans="1:4" ht="20" customHeight="1">
       <c r="A15" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>28</v>
@@ -1036,7 +1073,7 @@
     </row>
     <row r="16" spans="1:4" ht="20" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>30</v>
@@ -1050,7 +1087,7 @@
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>31</v>
@@ -1064,142 +1101,154 @@
     </row>
     <row r="18" spans="1:4" ht="20" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="5">
+        <v>805</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="C18" s="5">
-        <v>805</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="20" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5">
         <v>805</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5">
         <v>805</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="5">
         <v>805</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>42</v>
+        <v>69</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="C22" s="5">
         <v>805</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C23" s="5">
         <v>805</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="25" spans="1:4" ht="20" customHeight="1">
-      <c r="A25" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>50</v>
+      <c r="A25" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="16" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="20" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="20" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>73</v>
+        <v>49</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>78</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="20" customHeight="1">
+      <c r="A28" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
125B Rev 4 PCB
Updated hardware design for the 125B PCB to include hardware muting.  This allows the signal to be muted during true bypass relay switching, which reduces any popping that might happen otherwise.

Updated the example software to use the hardware mute when using the bypass.  Also, added basic menu support to the OLED screen with some settings for the Tremolo and hardware device.
</commit_message>
<xml_diff>
--- a/GuitarPedal125b/pcb/BOM_JLCSMT_DaisySeedGuitarPedal125b.xlsx
+++ b/GuitarPedal125b/pcb/BOM_JLCSMT_DaisySeedGuitarPedal125b.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshep/Dev/DaisySeedProjects/GuitarPedal125b/pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAE0C70-2DCE-CB4F-BBD6-56C1240D3B6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ECD584-DFAB-8E41-9007-B3A435A27898}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68540" yWindow="3140" windowWidth="28800" windowHeight="21660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68540" yWindow="3100" windowWidth="28800" windowHeight="21660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
   <si>
     <t>Comment</t>
   </si>
@@ -102,9 +102,6 @@
     <t>10nF</t>
   </si>
   <si>
-    <t>C18-21</t>
-  </si>
-  <si>
     <t>C1710</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>SS8050</t>
   </si>
   <si>
-    <t>R22-29</t>
-  </si>
-  <si>
     <t>2M</t>
   </si>
   <si>
@@ -309,9 +303,6 @@
     <t>R15</t>
   </si>
   <si>
-    <t>R19, R20, R21</t>
-  </si>
-  <si>
     <t>C78589</t>
   </si>
   <si>
@@ -334,6 +325,27 @@
   </si>
   <si>
     <t>C5377809</t>
+  </si>
+  <si>
+    <t>SOP-4-2.54mm</t>
+  </si>
+  <si>
+    <t>U7, U8</t>
+  </si>
+  <si>
+    <t>R19, R20, R21, R24, R25</t>
+  </si>
+  <si>
+    <t>R22, R23, R26, R27</t>
+  </si>
+  <si>
+    <t>C18, C19</t>
+  </si>
+  <si>
+    <t>CPC1018N</t>
+  </si>
+  <si>
+    <t>C1558973</t>
   </si>
 </sst>
 </file>
@@ -458,7 +470,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -508,6 +520,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -853,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>
@@ -927,328 +942,342 @@
       <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="5">
+        <v>805</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="5">
-        <v>805</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
       <c r="A13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="C13" s="5">
+        <v>805</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C13" s="5">
-        <v>805</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>26</v>
-      </c>
       <c r="D14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="20" customHeight="1">
       <c r="A15" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="5">
         <v>805</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="20" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="5">
         <v>805</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5">
+        <v>805</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" s="5">
-        <v>805</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="20" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" s="5">
         <v>805</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="20" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="5">
         <v>805</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="5">
         <v>805</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="5">
         <v>805</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C22" s="5">
         <v>805</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="C23" s="5">
         <v>805</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="20" customHeight="1">
       <c r="A25" s="14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="20" customHeight="1">
       <c r="A26" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="20" customHeight="1">
       <c r="A27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="20" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="20" customHeight="1">
+      <c r="A29" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>